<commit_message>
Arnold Herrera: Se añade dataset, dividido en training, data y las imagenes originales del experimento, también se actualiza el cronograma
</commit_message>
<xml_diff>
--- a/MusicalFigureDetection Schedule.xlsx
+++ b/MusicalFigureDetection Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositories GitHub\MusicalFigureDetection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F88055C2-E0F8-4263-A66E-C4ABC1515075}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CF7597-26B8-45B7-89AC-F71B381E4BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EB8AC08-26EA-4D7F-8DDD-D17B35E33653}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Entrenamient</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>MusicalFigureDetection Schedule</t>
+  </si>
+  <si>
+    <t>Configuración tarjeta gráfica</t>
   </si>
 </sst>
 </file>
@@ -106,11 +109,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,65 +428,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D42FD14-723E-4073-B27A-12D45E58D4E1}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>44093</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
-        <v>44100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="2">
+        <v>44102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3">
-        <f>B3+15</f>
-        <v>44115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2">
+        <v>44114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3">
-        <f>B4+15</f>
-        <v>44130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="2">
+        <v>44128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
-        <f>B5+15</f>
-        <v>44145</v>
+      <c r="B7" s="2">
+        <v>44142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>